<commit_message>
more updates and corrected excel file
</commit_message>
<xml_diff>
--- a/CPAC2019.xlsx
+++ b/CPAC2019.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiamulette/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDF38BE-298E-3741-91EF-52A2D7F17218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDCF66B-3584-FE4D-AD4E-9760314EAB7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{0A6D2ECA-6478-934D-8685-75FBDF416AEB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="239">
   <si>
     <t>Event Title</t>
   </si>
@@ -746,6 +746,9 @@
   </si>
   <si>
     <t>Panels</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1:00:00 PM</t>
   </si>
 </sst>
 </file>
@@ -1143,8 +1146,8 @@
   <dimension ref="A1:I994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1353,11 +1356,15 @@
         <v>13</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="11">
+        <v>43583</v>
+      </c>
       <c r="E8" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F8" s="5"/>
+        <v>238</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>237</v>
       </c>
@@ -1376,9 +1383,11 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F9" s="8"/>
+        <v>238</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>237</v>
       </c>
@@ -1396,9 +1405,11 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>238</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>237</v>
       </c>
@@ -1417,9 +1428,11 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>238</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>237</v>
       </c>
@@ -1438,9 +1451,11 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>238</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>237</v>
       </c>
@@ -1459,9 +1474,11 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>238</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>237</v>
       </c>
@@ -1506,10 +1523,12 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F15" s="5"/>
+      <c r="E15" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>237</v>
       </c>
@@ -1527,10 +1546,12 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F16" s="5"/>
+      <c r="E16" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>237</v>
       </c>
@@ -1575,10 +1596,12 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F18" s="5"/>
+      <c r="E18" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>237</v>
       </c>
@@ -1596,10 +1619,12 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F19" s="5"/>
+      <c r="E19" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G19" s="1" t="s">
         <v>237</v>
       </c>
@@ -1642,10 +1667,12 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F21" s="5"/>
+      <c r="E21" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>237</v>
       </c>
@@ -1693,7 +1720,9 @@
       <c r="E23" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>237</v>
       </c>
@@ -1790,9 +1819,15 @@
         <v>50</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="D27" s="11">
+        <v>43583</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.55208333333333337</v>
+      </c>
       <c r="G27" s="1" t="s">
         <v>237</v>
       </c>
@@ -1836,9 +1871,15 @@
         <v>54</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="D29" s="11">
+        <v>43583</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.63541666666666663</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>237</v>
       </c>
@@ -1880,9 +1921,15 @@
         <v>58</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="D31" s="11">
+        <v>43583</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0.61458333333333337</v>
+      </c>
       <c r="G31" s="1" t="s">
         <v>237</v>
       </c>
@@ -1954,8 +2001,12 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="5"/>
+      <c r="E34" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>237</v>
       </c>
@@ -1973,8 +2024,12 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="E35" s="6">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.6875</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>237</v>
       </c>
@@ -1992,8 +2047,12 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="E36" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0.72916666666666696</v>
+      </c>
       <c r="G36" s="1" t="s">
         <v>237</v>
       </c>
@@ -2011,8 +2070,12 @@
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="6">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0.77083333333333304</v>
+      </c>
       <c r="G37" s="1" t="s">
         <v>237</v>
       </c>
@@ -2029,8 +2092,12 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="E38" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G38" s="1" t="s">
         <v>237</v>
       </c>
@@ -2048,8 +2115,12 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="E39" s="6">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.6875</v>
+      </c>
       <c r="G39" s="1" t="s">
         <v>237</v>
       </c>
@@ -2067,8 +2138,12 @@
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="E40" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0.72916666666666696</v>
+      </c>
       <c r="G40" s="1" t="s">
         <v>237</v>
       </c>
@@ -2086,8 +2161,12 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="E41" s="6">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.77083333333333304</v>
+      </c>
       <c r="G41" s="1" t="s">
         <v>237</v>
       </c>
@@ -2132,8 +2211,12 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="E43" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G43" s="1" t="s">
         <v>237</v>
       </c>
@@ -2151,8 +2234,12 @@
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="E44" s="6">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0.6875</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>237</v>
       </c>
@@ -2170,8 +2257,12 @@
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="E45" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0.72916666666666696</v>
+      </c>
       <c r="G45" s="1" t="s">
         <v>237</v>
       </c>
@@ -2189,8 +2280,12 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="E46" s="6">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0.77083333333333304</v>
+      </c>
       <c r="G46" s="1" t="s">
         <v>237</v>
       </c>
@@ -2235,8 +2330,12 @@
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="E48" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="F48" s="6">
+        <v>0.63541666666666663</v>
+      </c>
       <c r="G48" s="1" t="s">
         <v>237</v>
       </c>
@@ -2254,8 +2353,12 @@
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="E49" s="6">
+        <v>0.63541666666666696</v>
+      </c>
+      <c r="F49" s="6">
+        <v>0.67708333333333304</v>
+      </c>
       <c r="G49" s="1" t="s">
         <v>237</v>
       </c>
@@ -2273,8 +2376,12 @@
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="E50" s="6">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="F50" s="6">
+        <v>0.71875</v>
+      </c>
       <c r="G50" s="1" t="s">
         <v>237</v>
       </c>
@@ -2346,8 +2453,12 @@
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="E53" s="6">
+        <v>0.65625</v>
+      </c>
+      <c r="F53" s="6">
+        <v>0.69791666666666663</v>
+      </c>
       <c r="G53" s="1" t="s">
         <v>237</v>
       </c>
@@ -2365,8 +2476,12 @@
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="E54" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="F54" s="6">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>237</v>
       </c>
@@ -2384,8 +2499,12 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="E55" s="6">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="F55" s="6">
+        <v>0.55208333333333304</v>
+      </c>
       <c r="G55" s="1" t="s">
         <v>237</v>
       </c>
@@ -2403,8 +2522,12 @@
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="E56" s="6">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="F56" s="6">
+        <v>0.59375</v>
+      </c>
       <c r="G56" s="1" t="s">
         <v>237</v>
       </c>
@@ -2422,8 +2545,12 @@
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
+      <c r="E57" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="F57" s="6">
+        <v>0.63541666666666696</v>
+      </c>
       <c r="G57" s="1" t="s">
         <v>237</v>
       </c>
@@ -2468,8 +2595,12 @@
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="E59" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="F59" s="6">
+        <v>0.72916666666666696</v>
+      </c>
       <c r="G59" s="1" t="s">
         <v>237</v>
       </c>
@@ -2487,8 +2618,12 @@
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="E60" s="6">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="F60" s="6">
+        <v>0.77083333333333304</v>
+      </c>
       <c r="G60" s="1" t="s">
         <v>237</v>
       </c>
@@ -2506,8 +2641,12 @@
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+      <c r="E61" s="6">
+        <v>0.77083333333333304</v>
+      </c>
+      <c r="F61" s="6">
+        <v>0.8125</v>
+      </c>
       <c r="G61" s="1" t="s">
         <v>237</v>
       </c>
@@ -2552,8 +2691,12 @@
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
+      <c r="E63" s="6">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="F63" s="6">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="G63" s="1" t="s">
         <v>237</v>
       </c>
@@ -2571,8 +2714,12 @@
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
+      <c r="E64" s="6">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="F64" s="6">
+        <v>0.65625</v>
+      </c>
       <c r="G64" s="1" t="s">
         <v>237</v>
       </c>
@@ -2589,8 +2736,12 @@
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="E65" s="6">
+        <v>0.65625</v>
+      </c>
+      <c r="F65" s="6">
+        <v>0.69791666666666663</v>
+      </c>
       <c r="G65" s="1" t="s">
         <v>237</v>
       </c>
@@ -2608,8 +2759,12 @@
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+      <c r="E66" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="F66" s="6">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="G66" s="1" t="s">
         <v>237</v>
       </c>
@@ -2627,8 +2782,12 @@
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+      <c r="E67" s="6">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="F67" s="6">
+        <v>0.55208333333333304</v>
+      </c>
       <c r="G67" s="1" t="s">
         <v>237</v>
       </c>
@@ -2646,8 +2805,12 @@
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+      <c r="E68" s="6">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="F68" s="6">
+        <v>0.59375</v>
+      </c>
       <c r="G68" s="1" t="s">
         <v>237</v>
       </c>
@@ -2665,8 +2828,12 @@
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="E69" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="F69" s="6">
+        <v>0.63541666666666696</v>
+      </c>
       <c r="G69" s="1" t="s">
         <v>237</v>
       </c>
@@ -2684,8 +2851,12 @@
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="E70" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F70" s="6">
+        <v>0.6875</v>
+      </c>
       <c r="G70" s="1" t="s">
         <v>237</v>
       </c>
@@ -2703,8 +2874,12 @@
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
+      <c r="E71" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="F71" s="6">
+        <v>0.72916666666666696</v>
+      </c>
       <c r="G71" s="1" t="s">
         <v>237</v>
       </c>
@@ -2722,8 +2897,12 @@
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="E72" s="6">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="F72" s="6">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="G72" s="1" t="s">
         <v>237</v>
       </c>
@@ -2741,8 +2920,12 @@
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+      <c r="E73" s="6">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="F73" s="6">
+        <v>0.65625</v>
+      </c>
       <c r="G73" s="1" t="s">
         <v>237</v>
       </c>
@@ -2760,8 +2943,12 @@
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="E74" s="6">
+        <v>0.65625</v>
+      </c>
+      <c r="F74" s="6">
+        <v>0.69791666666666663</v>
+      </c>
       <c r="G74" s="1" t="s">
         <v>237</v>
       </c>
@@ -2806,8 +2993,12 @@
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+      <c r="E76" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F76" s="6">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="G76" s="1" t="s">
         <v>237</v>
       </c>
@@ -2825,8 +3016,12 @@
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="E77" s="6">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="F77" s="4">
+        <v>0.48958333333333331</v>
+      </c>
       <c r="G77" s="1" t="s">
         <v>237</v>
       </c>
@@ -2847,10 +3042,10 @@
         <v>43582</v>
       </c>
       <c r="E78" s="5">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="F78" s="5">
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>227</v>
@@ -3663,7 +3858,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="F111" s="10">
-        <v>6.25E-2</v>
+        <v>0.5625</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>223</v>
@@ -3688,7 +3883,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="F112" s="10">
-        <v>0.1875</v>
+        <v>0.6875</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>223</v>
@@ -3713,7 +3908,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F113" s="10">
-        <v>0.3125</v>
+        <v>0.8125</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>223</v>
@@ -3738,7 +3933,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="F114" s="10">
-        <v>6.25E-2</v>
+        <v>0.5625</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>223</v>
@@ -3763,7 +3958,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="F115" s="10">
-        <v>0.1875</v>
+        <v>0.6875</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>223</v>
@@ -3788,7 +3983,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F116" s="10">
-        <v>0.3125</v>
+        <v>0.8125</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>223</v>

</xml_diff>